<commit_message>
Fix groups and check all posts
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -401,563 +401,997 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>Мария Юрова</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>306803045</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>https://vk.com/id306803045</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Олег Поташов</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>485198464</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>https://vk.com/id485198464</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Всеволод Коваленко</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>582038896</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>https://vk.com/id582038896</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Веду Дневник по Вебу (ВДВ)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>212637974</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://vk.com/id212637974</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Даниил Хохлов</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>463026941</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>https://vk.com/id463026941</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Евгений Новожилов</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>513145873</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>https://vk.com/id513145873</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Вадим Кузьмин</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>542063563</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>https://vk.com/id542063563</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Света Чернокуцатова</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>126071013</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>https://vk.com/id126071013</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Виктория Шубина</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>306230404</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>https://vk.com/id306230404</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Михаил Кириллов</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>198672105</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>https://vk.com/id198672105</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Саша Халудоров</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>659091073</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>https://vk.com/id659091073</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Николай Толстов</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>685751155</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>https://vk.com/id685751155</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Qqq Www</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>62608138</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>https://vk.com/id62608138</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Эдуард Кузнецов</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>395886397</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>https://vk.com/id395886397</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Дима Малиев</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>588155639</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>https://vk.com/id588155639</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Igor Shlyakov</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>234063598</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>https://vk.com/id234063598</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Алексей Гакман</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>11721597</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>https://vk.com/id11721597</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Женя Михайлов</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>231936063</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>https://vk.com/id231936063</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Олег Смородников</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>275944431</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
         <is>
           <t>https://vk.com/id275944431</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Ахмадали Алимов</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>475870319</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>https://vk.com/id475870319</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Виктор Резнов</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>497213918</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>https://vk.com/id497213918</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Никита Холодняк</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>591561323</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>https://vk.com/id591561323</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Рома Жарков</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>171745503</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
         <is>
           <t>https://vk.com/id171745503</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>Эльдар Кузяев</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>7475909</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>https://vk.com/id7475909</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Максим Комаров</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>199124895</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
         <is>
           <t>https://vk.com/id199124895</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="n">
+        <v>26</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Graf Monte-Cristo</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>503149131</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
         <is>
           <t>https://vk.com/id503149131</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Александр Ливанов</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>550097213</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
         <is>
           <t>https://vk.com/id550097213</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Вениамин Шкуратов</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>735503783</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
         <is>
           <t>https://vk.com/id735503783</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Дмитрий Глянцев</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>714496054</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>https://vk.com/id714496054</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Андрей Алымов</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>71969366</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>https://vk.com/id71969366</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Виктория Кусь</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>221615664</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>https://vk.com/id221615664</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Артем К-В</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>315676571</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>https://vk.com/id315676571</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Максим Фомичев</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>208855427</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>https://vk.com/id208855427</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Александр Щербаков</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>445138397</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
         <is>
           <t>https://vk.com/id445138397</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="35">
+      <c r="A35" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Юрий Захаров</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>530204469</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
         <is>
           <t>https://vk.com/id530204469</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Vladimir Gloohoff</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>162180769</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
         <is>
           <t>https://vk.com/id162180769</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="37">
+      <c r="A37" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Николай Туренко</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>183816785</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
         <is>
           <t>https://vk.com/id183816785</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Elder Bagaytdinov</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>617925729</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
         <is>
           <t>https://vk.com/id617925729</t>
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>Юрий Гужиев</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>26472214</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
         <is>
           <t>https://vk.com/id26472214</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="40">
+      <c r="A40" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Илья Викторов</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>146124357</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
         <is>
           <t>https://vk.com/id146124357</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Джеймс Рейнор</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>712499475</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
         <is>
           <t>https://vk.com/id712499475</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="42">
+      <c r="A42" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Дарья Генералова</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>474494205</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
         <is>
           <t>https://vk.com/id474494205</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="43">
+      <c r="A43" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Савелий Фурсов</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>420782945</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
         <is>
           <t>https://vk.com/id420782945</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>Рустэм Шакиров</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>12748513</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
         <is>
           <t>https://vk.com/id12748513</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="45">
+      <c r="A45" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Илья Опарин</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>223200636</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
         <is>
           <t>https://vk.com/id223200636</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="46">
+      <c r="A46" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Антон Процун</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>560517052</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
         <is>
           <t>https://vk.com/id560517052</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="47">
+      <c r="A47" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Алексей Дьяков</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>153404055</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
         <is>
           <t>https://vk.com/id153404055</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Дарина Гарская</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>360364958</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://vk.com/id360364958</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Дмитрий Попов</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>613007793</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://vk.com/id613007793</t>
         </is>
       </c>
     </row>

</xml_diff>